<commit_message>
Added basis for hit-scan shooting and health
</commit_message>
<xml_diff>
--- a/Castle Defender/Assets/To do.xlsx
+++ b/Castle Defender/Assets/To do.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Lowest Priority</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>&gt; Have a lift to lower the player down from the wall between rounds.</t>
+  </si>
+  <si>
+    <t>Mute music with 'M'</t>
+  </si>
+  <si>
+    <t>Weather effects e.g. rain</t>
   </si>
 </sst>
 </file>
@@ -500,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,6 +600,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -610,13 +619,16 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated To do and README
Added new ideas, rearranged priorities, and formatted to reflect degree
of implementation.
</commit_message>
<xml_diff>
--- a/Castle Defender/Assets/To do.xlsx
+++ b/Castle Defender/Assets/To do.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Lowest Priority</t>
   </si>
@@ -114,13 +114,28 @@
   </si>
   <si>
     <t>Weather effects e.g. rain</t>
+  </si>
+  <si>
+    <t>Fully implemented</t>
+  </si>
+  <si>
+    <t>Partially implemented</t>
+  </si>
+  <si>
+    <t>Not implemented</t>
+  </si>
+  <si>
+    <t>Sprinting with Shift</t>
+  </si>
+  <si>
+    <t>Create a sniper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +159,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +197,16 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -198,24 +237,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -504,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,11 +561,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -537,10 +582,10 @@
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -548,7 +593,7 @@
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
@@ -570,7 +615,7 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C6" t="s">
@@ -584,13 +629,13 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -601,18 +646,21 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="A10" t="s">
         <v>20</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -620,15 +668,33 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
       <c r="C12" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Todo and README
Added latest build to README.
</commit_message>
<xml_diff>
--- a/Castle Defender/Assets/To do.xlsx
+++ b/Castle Defender/Assets/To do.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Lowest Priority</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Create a sniper</t>
+  </si>
+  <si>
+    <t>Make recoil/accuracy dependent on whether or not player is standing still.</t>
   </si>
 </sst>
 </file>
@@ -552,7 +555,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +599,7 @@
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -604,7 +607,7 @@
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
@@ -626,7 +629,7 @@
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -680,6 +683,11 @@
       </c>
       <c r="C12" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated README and Todo
</commit_message>
<xml_diff>
--- a/Castle Defender/Assets/To do.xlsx
+++ b/Castle Defender/Assets/To do.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Features" sheetId="1" r:id="rId1"/>
+    <sheet name="Bugs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Lowest Priority</t>
   </si>
@@ -132,6 +133,21 @@
   </si>
   <si>
     <t>Make recoil/accuracy dependent on whether or not player is standing still.</t>
+  </si>
+  <si>
+    <t>Be able to switch weapons mid-reload.</t>
+  </si>
+  <si>
+    <t>Prevent player from rotating camera too far.</t>
+  </si>
+  <si>
+    <t>Re-lock cursor to screen after tabbing out and tabbing back in.</t>
+  </si>
+  <si>
+    <t>On loss, repeatedly pausing/unpausing causes the games to run for ~1 frame</t>
+  </si>
+  <si>
+    <t>If switch weapon before finish reloading, and switch back, the weapon model transform is odd.</t>
   </si>
 </sst>
 </file>
@@ -247,7 +263,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1"/>
@@ -255,6 +271,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -564,11 +590,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -670,7 +696,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -702,6 +728,156 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="77.5703125" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3" s="12" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Todo and README with latest build
</commit_message>
<xml_diff>
--- a/Castle Defender/Assets/To do.xlsx
+++ b/Castle Defender/Assets/To do.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Features" sheetId="1" r:id="rId1"/>
-    <sheet name="Bugs" sheetId="2" r:id="rId2"/>
+    <sheet name="Immediate Checklist" sheetId="3" r:id="rId1"/>
+    <sheet name="Features" sheetId="1" r:id="rId2"/>
+    <sheet name="Bugs and Quirks" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Lowest Priority</t>
   </si>
@@ -132,9 +133,6 @@
     <t>Create a sniper</t>
   </si>
   <si>
-    <t>Make recoil/accuracy dependent on whether or not player is standing still.</t>
-  </si>
-  <si>
     <t>Be able to switch weapons mid-reload.</t>
   </si>
   <si>
@@ -148,6 +146,33 @@
   </si>
   <si>
     <t>If switch weapon before finish reloading, and switch back, the weapon model transform is odd.</t>
+  </si>
+  <si>
+    <t>Be able to shoot bullets immediately after switching guns regardless whether or not you're reloading.</t>
+  </si>
+  <si>
+    <t>Zoom out when reloading.</t>
+  </si>
+  <si>
+    <t>Add aim down sights animation</t>
+  </si>
+  <si>
+    <t>Add an indicator for when you can fire again</t>
+  </si>
+  <si>
+    <t>Make recoil/accuracy dependent on whether or not player is standing still</t>
+  </si>
+  <si>
+    <t>Add sniper rifle purchase button</t>
+  </si>
+  <si>
+    <t>Add sniper rifle ammo button</t>
+  </si>
+  <si>
+    <t>Make the sniper rifle zoom out when firing</t>
+  </si>
+  <si>
+    <t>When switching weapons while reloading, cancel reload and allow to fire immediately</t>
   </si>
 </sst>
 </file>
@@ -263,7 +288,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1"/>
@@ -281,6 +306,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -578,163 +606,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="77.5703125" customWidth="1"/>
+    <col min="1" max="1" width="77.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -744,7 +652,176 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="77.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,11 +831,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" s="12" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
@@ -773,42 +850,44 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated To do and README with latest build
</commit_message>
<xml_diff>
--- a/Castle Defender/Assets/To do.xlsx
+++ b/Castle Defender/Assets/To do.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Immediate Checklist" sheetId="3" r:id="rId1"/>
-    <sheet name="Features" sheetId="1" r:id="rId2"/>
-    <sheet name="Bugs and Quirks" sheetId="2" r:id="rId3"/>
+    <sheet name="Features" sheetId="1" r:id="rId1"/>
+    <sheet name="Bugs and Quirks" sheetId="2" r:id="rId2"/>
+    <sheet name="Immediate Checklist" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Lowest Priority</t>
   </si>
@@ -148,12 +148,6 @@
     <t>If switch weapon before finish reloading, and switch back, the weapon model transform is odd.</t>
   </si>
   <si>
-    <t>Be able to shoot bullets immediately after switching guns regardless whether or not you're reloading.</t>
-  </si>
-  <si>
-    <t>Zoom out when reloading.</t>
-  </si>
-  <si>
     <t>Add aim down sights animation</t>
   </si>
   <si>
@@ -163,16 +157,10 @@
     <t>Make recoil/accuracy dependent on whether or not player is standing still</t>
   </si>
   <si>
-    <t>Add sniper rifle purchase button</t>
-  </si>
-  <si>
-    <t>Add sniper rifle ammo button</t>
-  </si>
-  <si>
-    <t>Make the sniper rifle zoom out when firing</t>
-  </si>
-  <si>
-    <t>When switching weapons while reloading, cancel reload and allow to fire immediately</t>
+    <t>Player moves slightly when standing still.</t>
+  </si>
+  <si>
+    <t>Player can by-pass nextFire wait time on sniper rifle by quickly switching to another weapon and switching back and firing.</t>
   </si>
 </sst>
 </file>
@@ -606,49 +594,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="77.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -768,7 +713,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>34</v>
@@ -779,7 +724,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -790,7 +735,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -816,12 +761,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +808,9 @@
       <c r="B4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -875,15 +822,13 @@
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -966,4 +911,32 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="77.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>